<commit_message>
weapon spreadsheets stat change
increased amour pen for AP and HE
corrected incorrect shield damage values
</commit_message>
<xml_diff>
--- a/exo_2.0_mod_rework/Combat/weapon spreadsheet.xlsx
+++ b/exo_2.0_mod_rework/Combat/weapon spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\ExOverhaul\2.0_mod_rework\Combat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A606463D-631F-4011-9CD9-432B0A5F6EC2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91389490-9A68-4131-914B-8B9C7542FD0D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2" xr2:uid="{B0C87D61-94C4-4543-8456-C868BBB37C70}"/>
   </bookViews>
@@ -1470,7 +1470,7 @@
   <dimension ref="A2:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,10 +1586,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="2">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="L9" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M9" s="2">
         <v>0</v>
@@ -1630,10 +1630,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="2">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="L10" s="2">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="M10" s="2">
         <v>0</v>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="L11" s="2">
         <v>0</v>
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>-0.7</v>
+        <v>-1</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
@@ -1762,10 +1762,10 @@
         <v>0</v>
       </c>
       <c r="K13" s="2">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="L13" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
@@ -1806,10 +1806,10 @@
         <v>0</v>
       </c>
       <c r="K14" s="2">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="L14" s="2">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="M14" s="2">
         <v>0</v>
@@ -1850,7 +1850,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="L15" s="2">
         <v>0</v>
@@ -1894,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="2">
-        <v>-0.7</v>
+        <v>-1</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
@@ -1938,10 +1938,10 @@
         <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="L17" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M17" s="2">
         <v>0</v>
@@ -1982,10 +1982,10 @@
         <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="L18" s="2">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="M18" s="2">
         <v>0</v>
@@ -2026,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="L19" s="2">
         <v>0</v>
@@ -2070,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="2">
-        <v>-0.7</v>
+        <v>-1</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
@@ -2114,10 +2114,10 @@
         <v>0</v>
       </c>
       <c r="K21" s="2">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="L21" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M21" s="2">
         <v>0</v>
@@ -2158,10 +2158,10 @@
         <v>0</v>
       </c>
       <c r="K22" s="2">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="L22" s="2">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="M22" s="2">
         <v>0</v>
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="L23" s="2">
         <v>0</v>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="2">
-        <v>-0.7</v>
+        <v>-1</v>
       </c>
       <c r="L24" s="2">
         <v>0</v>

</xml_diff>